<commit_message>
updated test for sprint 2
</commit_message>
<xml_diff>
--- a/files/Documents/Team 4 Documents/sprint2_team4_xlsx_no_pii.xlsx
+++ b/files/Documents/Team 4 Documents/sprint2_team4_xlsx_no_pii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingt\Documents\comp410\comp410_summer_2022\files\Documents\Team 4 Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFD7421B-E500-47A9-8A74-E346F9B04C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E06D3183-F42F-466D-ADF1-14566B915355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9516" yWindow="1140" windowWidth="13452" windowHeight="11100" xr2:uid="{EA188841-311B-4C2E-ACEA-BD5A4B2FCB08}"/>
+    <workbookView xWindow="9588" yWindow="1140" windowWidth="13452" windowHeight="11100" xr2:uid="{EA188841-311B-4C2E-ACEA-BD5A4B2FCB08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>